<commit_message>
Added Github Links to BOM
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/Camera_Adapter_Logitech_BOM.xlsx
+++ b/Documentation/Working_Documents/Camera_Adapter_Logitech_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-Team/Shared Documents/Server/3 AT Library/WIP/Camera Mount Adapter for Logitech Adaptive Gaming/GitHub/Documentation/Working_Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tazo\Documents\GitHub\Camera-Mount-Adapter-for-Logitech-Adaptive-Gaming\Documentation\Working_Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{693E7A0C-54B8-4EA0-AAFA-4254073F1F1F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FAD733-1024-486D-8A6A-499535731EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,6 @@
     <t xml:space="preserve">The adapter for the 1/4"-20 threads which can be attached to a button from the Logitech Adaptive Gaming Kit. </t>
   </si>
   <si>
-    <t>Add Github link</t>
-  </si>
-  <si>
     <t>Total Print Cost:</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>1/4" - 20 Barbed T-Nut 5/16" barrel length.</t>
+  </si>
+  <si>
+    <t>Camera-Mount-Adapters-for-the-Logitech-Adaptive-Gaming-Kit/Build_Files at main · makersmakingchange/Camera-Mount-Adapters-for-the-Logitech-Adaptive-Gaming-Kit (github.com)</t>
   </si>
 </sst>
 </file>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="C22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -892,7 +892,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -998,14 +998,14 @@
       <c r="F10">
         <v>71</v>
       </c>
-      <c r="G10" s="26" t="s">
-        <v>28</v>
+      <c r="G10" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="D11" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="19">
         <f>SUM(E10:E10)</f>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -1030,17 +1030,17 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1056,7 +1056,7 @@
     </row>
     <row r="17" spans="1:10" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="4">
@@ -1110,7 +1110,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20">
         <v>12</v>
@@ -1197,10 +1197,10 @@
     </row>
     <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="25" t="s">
         <v>35</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>36</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -1215,16 +1215,16 @@
       <c r="F24">
         <v>219</v>
       </c>
-      <c r="G24" s="26" t="s">
-        <v>28</v>
+      <c r="G24" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="25" t="s">
         <v>37</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>38</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -1243,10 +1243,10 @@
     </row>
     <row r="26" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="25" t="s">
         <v>39</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>40</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -1265,10 +1265,10 @@
     </row>
     <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="25" t="s">
         <v>41</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>42</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -1288,7 +1288,7 @@
     <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11"/>
       <c r="D28" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E28" s="19">
         <f>SUM(E24:E27)</f>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -1312,17 +1312,17 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1334,21 +1334,21 @@
     <hyperlink ref="H6" r:id="rId2" xr:uid="{8613809C-52EA-405F-BB72-DEB4F63981AF}"/>
     <hyperlink ref="H21" r:id="rId3" xr:uid="{DED601A8-6248-4A01-8F16-7222D48AA641}"/>
     <hyperlink ref="H20" r:id="rId4" xr:uid="{198AB59F-D6CB-40FB-9AAC-CA3097ABCCB3}"/>
+    <hyperlink ref="G24" r:id="rId5" display="https://github.com/makersmakingchange/Camera-Mount-Adapters-for-the-Logitech-Adaptive-Gaming-Kit/tree/main/Build_Files" xr:uid="{61210271-135D-4FBF-9153-C82563442979}"/>
+    <hyperlink ref="G10" r:id="rId6" display="https://github.com/makersmakingchange/Camera-Mount-Adapters-for-the-Logitech-Adaptive-Gaming-Kit/tree/main/Build_Files" xr:uid="{BBA2CF49-0ED9-4F21-9FB4-4C056A7E0BEE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1589,21 +1589,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
-    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1628,9 +1627,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
+    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>